<commit_message>
updates to UI and functionality
</commit_message>
<xml_diff>
--- a/xseller8-backend/central_spreadsheet.xlsx
+++ b/xseller8-backend/central_spreadsheet.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -427,9 +427,49 @@
         <v>Total</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2024-10-10</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Example Company</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Item 1</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2024-10-10</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Example Company</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Item 2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -461,7 +501,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -474,9 +514,25 @@
         <v>Current Price</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Item 1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Item 2</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing errors with UI
</commit_message>
<xml_diff>
--- a/xseller8-backend/central_spreadsheet.xlsx
+++ b/xseller8-backend/central_spreadsheet.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -467,9 +467,23 @@
         <v>600</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2024-10-10</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Sample Item</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>12.5</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -501,7 +515,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -530,9 +544,17 @@
         <v>200</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Sample Item</v>
+      </c>
+      <c r="B4">
+        <v>12.5</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>